<commit_message>
prefecture 2012, 2013 data
</commit_message>
<xml_diff>
--- a/raw_data/All 2008, 2009, 2010 data by week and location.xlsx
+++ b/raw_data/All 2008, 2009, 2010 data by week and location.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1863,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="BB3" sqref="BB3:BB50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>